<commit_message>
new TrainingData (> 1000)
</commit_message>
<xml_diff>
--- a/backend/model_data/TrainingData_5cat_de.xlsx
+++ b/backend/model_data/TrainingData_5cat_de.xlsx
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15279" uniqueCount="1528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15529" uniqueCount="1579">
   <si>
     <t>User</t>
   </si>
@@ -4705,6 +4705,159 @@
   </si>
   <si>
     <t>Länge VW Sharan (klassisches Familienauto) 4,80</t>
+  </si>
+  <si>
+    <t>So knapp, und doch alles gesagt!</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/politik/ausland/2019-11/bertelsmann-stiftung-studie-europaeische-union-buerger-umweltschutz</t>
+  </si>
+  <si>
+    <t>well said</t>
+  </si>
+  <si>
+    <t>Im allgemeinen haben Sie da recht, aber derartige Studien kommen seit einiger Zeit ziemlich konstant zu eben JENEM Ergebnis, ganz egal, wer sie durchführt</t>
+  </si>
+  <si>
+    <t>Nein, ich bleibe dabei.</t>
+  </si>
+  <si>
+    <t>Watzinger</t>
+  </si>
+  <si>
+    <t>Rofur</t>
+  </si>
+  <si>
+    <t>SpamBot</t>
+  </si>
+  <si>
+    <t>Ich fand das ziemlich deprimierend</t>
+  </si>
+  <si>
+    <t>Hanayagi</t>
+  </si>
+  <si>
+    <t>Allerdings kann auch Medienunterricht die Leute nicht intelligenter machen als sie sind</t>
+  </si>
+  <si>
+    <t>Deontos</t>
+  </si>
+  <si>
+    <t>Und das macht mir für zukünftige Wahlen durchaus Sorgen</t>
+  </si>
+  <si>
+    <t>Sie haben ja Recht</t>
+  </si>
+  <si>
+    <t>EinTollerName</t>
+  </si>
+  <si>
+    <t>Aber das gilt eben für die eigene Meinung und Blase in noch höherem Umfang</t>
+  </si>
+  <si>
+    <t>Stimme ihnen zu, wobei es da auch sehr auf das Thema ankommt</t>
+  </si>
+  <si>
+    <t>Autsch! Das hat gesessen..</t>
+  </si>
+  <si>
+    <t>rock_lobster</t>
+  </si>
+  <si>
+    <t>Das ist das beste Verfahren, das es gibt</t>
+  </si>
+  <si>
+    <t>https://www.zeit.de/wirtschaft/2019-11/mietpreisbremse-immobilienmarkt-wohnungsmarkt-wohnungspolitik</t>
+  </si>
+  <si>
+    <t>TXL</t>
+  </si>
+  <si>
+    <t>Finde die Art wie Manuel mit den Menschen umgeht und mit ihnen redet echt super</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=vogs4NzqI3Q</t>
+  </si>
+  <si>
+    <t>sexuality</t>
+  </si>
+  <si>
+    <t>SimonJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menschlich und dennoch fragend. </t>
+  </si>
+  <si>
+    <t>Super Reportage!</t>
+  </si>
+  <si>
+    <t>Simon J gebe ich dir absolut recht</t>
+  </si>
+  <si>
+    <t>PPAY Lifestyle</t>
+  </si>
+  <si>
+    <t>Hammer Reporter</t>
+  </si>
+  <si>
+    <t>Ehrlich und offen</t>
+  </si>
+  <si>
+    <t>Was ich gut finde ist das er ihm wirklich sagt wie schwer es ihm manchmal fällt mit ihm das Thema zu besprechen</t>
+  </si>
+  <si>
+    <t>Rainer maria Rilke</t>
+  </si>
+  <si>
+    <t>Sehe ich auch so!!</t>
+  </si>
+  <si>
+    <t>Zockerpycho19</t>
+  </si>
+  <si>
+    <t>einer der wenigen guten reporter vom y kollektiv</t>
+  </si>
+  <si>
+    <t>MrFRDW</t>
+  </si>
+  <si>
+    <t>Sondern konstruktive Kommentare</t>
+  </si>
+  <si>
+    <t>carrotsonmywaywardson</t>
+  </si>
+  <si>
+    <t>Größten Respekt an den freiwilligen Undercover-Mitarbeiter, der alles mit angesehen haben muss.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=FvJ3U4NH0X8&amp;list=PLmdw78dzzcvD3dvdKlcnptu29p58wwViU&amp;index=4&amp;t=0s</t>
+  </si>
+  <si>
+    <t>Danke dass diesem Thema Aufmerksamkeit geschenkt wird.</t>
+  </si>
+  <si>
+    <t>Ich bin hin und hergerissen, ob ich mir das Video angucken möchte</t>
+  </si>
+  <si>
+    <t>https://t3n.de/news/ohne-plan-b-gekuendigt-erfahrungen-1225370/?utm_source=pocket-newtab</t>
+  </si>
+  <si>
+    <t>Will ja nicht jammern aber es geht auch anders</t>
+  </si>
+  <si>
+    <t>Ich hab auch ohne Plan B gekündigt</t>
+  </si>
+  <si>
+    <t>Jetzt bin ich arbeitslos, fett und nicht mehr krankenversichert. Ich lebe vom eingemachten, denn ALG gibts nicht</t>
+  </si>
+  <si>
+    <t>0.0.8</t>
+  </si>
+  <si>
+    <t>Henning</t>
+  </si>
+  <si>
+    <t>work</t>
   </si>
 </sst>
 </file>
@@ -5110,12 +5263,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U985"/>
+  <dimension ref="B1:U1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="P1" colorId="8" zoomScale="115" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A967" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="O1" colorId="8" zoomScale="115" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A989" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="U985" sqref="U985"/>
+      <selection pane="bottomLeft" activeCell="P1012" sqref="P1012"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23288,7 +23441,7 @@
         <v>128</v>
       </c>
       <c r="Q367" s="1" t="s">
-        <v>1498</v>
+        <v>5</v>
       </c>
       <c r="R367" s="1" t="s">
         <v>620</v>
@@ -52742,7 +52895,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="977" spans="15:21" x14ac:dyDescent="0.2">
+    <row r="977" spans="3:21" x14ac:dyDescent="0.2">
       <c r="O977" t="s">
         <v>1488</v>
       </c>
@@ -52765,7 +52918,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="978" spans="15:21" x14ac:dyDescent="0.2">
+    <row r="978" spans="3:21" x14ac:dyDescent="0.2">
       <c r="O978" t="s">
         <v>1527</v>
       </c>
@@ -52788,7 +52941,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="979" spans="15:21" x14ac:dyDescent="0.2">
+    <row r="979" spans="3:21" x14ac:dyDescent="0.2">
       <c r="O979" t="s">
         <v>1489</v>
       </c>
@@ -52811,7 +52964,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="980" spans="15:21" x14ac:dyDescent="0.2">
+    <row r="980" spans="3:21" x14ac:dyDescent="0.2">
       <c r="O980" t="s">
         <v>1490</v>
       </c>
@@ -52834,7 +52987,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="981" spans="15:21" x14ac:dyDescent="0.2">
+    <row r="981" spans="3:21" x14ac:dyDescent="0.2">
       <c r="O981" t="s">
         <v>1491</v>
       </c>
@@ -52857,7 +53010,7 @@
         <v>1502</v>
       </c>
     </row>
-    <row r="982" spans="15:21" x14ac:dyDescent="0.2">
+    <row r="982" spans="3:21" x14ac:dyDescent="0.2">
       <c r="O982" t="s">
         <v>1492</v>
       </c>
@@ -52880,7 +53033,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="983" spans="15:21" x14ac:dyDescent="0.2">
+    <row r="983" spans="3:21" x14ac:dyDescent="0.2">
       <c r="O983" t="s">
         <v>1493</v>
       </c>
@@ -52903,7 +53056,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="984" spans="15:21" x14ac:dyDescent="0.2">
+    <row r="984" spans="3:21" x14ac:dyDescent="0.2">
       <c r="O984" t="s">
         <v>1494</v>
       </c>
@@ -52926,7 +53079,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="985" spans="15:21" x14ac:dyDescent="0.2">
+    <row r="985" spans="3:21" x14ac:dyDescent="0.2">
       <c r="O985" t="s">
         <v>1510</v>
       </c>
@@ -52947,6 +53100,810 @@
       </c>
       <c r="U985" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="986" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C986" s="1" t="s">
+        <v>1534</v>
+      </c>
+      <c r="D986" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L986" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="M986" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="O986" t="s">
+        <v>1528</v>
+      </c>
+      <c r="P986" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q986" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="R986" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="S986" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="T986" s="1" t="s">
+        <v>1505</v>
+      </c>
+      <c r="U986" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="987" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C987" s="1" t="s">
+        <v>1535</v>
+      </c>
+      <c r="D987" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M987" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="O987" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P987" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q987" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="R987" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="S987" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T987" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="U987" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="988" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C988" s="1" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D988" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M988" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="O988" t="s">
+        <v>1532</v>
+      </c>
+      <c r="P988" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q988" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R988" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="S988" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="T988" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U988" s="1" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="989" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C989" s="1" t="s">
+        <v>1537</v>
+      </c>
+      <c r="D989" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M989" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="O989" t="s">
+        <v>1536</v>
+      </c>
+      <c r="P989" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q989" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="R989" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="S989" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="T989" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="U989" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="990" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C990" s="1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D990" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M990" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="O990" t="s">
+        <v>1538</v>
+      </c>
+      <c r="P990" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q990" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="R990" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="S990" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="T990" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="U990" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="991" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C991" s="1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D991" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M991" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="O991" t="s">
+        <v>1540</v>
+      </c>
+      <c r="P991" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q991" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="R991" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="S991" s="1" t="s">
+        <v>1506</v>
+      </c>
+      <c r="T991" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="U991" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="992" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C992" s="1" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D992" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M992" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="O992" t="s">
+        <v>1541</v>
+      </c>
+      <c r="P992" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q992" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="R992" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S992" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="T992" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="U992" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="993" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C993" s="1" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D993" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M993" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="O993" t="s">
+        <v>1543</v>
+      </c>
+      <c r="P993" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q993" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="R993" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="S993" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="T993" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="U993" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="994" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C994" s="1" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D994" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M994" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="O994" t="s">
+        <v>1544</v>
+      </c>
+      <c r="P994" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q994" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="R994" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="S994" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="T994" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="U994" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="995" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C995" s="1" t="s">
+        <v>1546</v>
+      </c>
+      <c r="D995" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M995" s="1" t="s">
+        <v>1529</v>
+      </c>
+      <c r="O995" t="s">
+        <v>1545</v>
+      </c>
+      <c r="P995" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q995" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="R995" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="S995" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="T995" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="U995" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="996" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C996" s="1" t="s">
+        <v>1549</v>
+      </c>
+      <c r="D996" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="M996" s="1" t="s">
+        <v>1548</v>
+      </c>
+      <c r="O996" t="s">
+        <v>1547</v>
+      </c>
+      <c r="P996" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q996" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="R996" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S996" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="T996" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="U996" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="997" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C997" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D997" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="M997" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="O997" t="s">
+        <v>1550</v>
+      </c>
+      <c r="P997" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q997" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="R997" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S997" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="T997" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="U997" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="998" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C998" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D998" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="M998" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="O998" t="s">
+        <v>1554</v>
+      </c>
+      <c r="P998" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q998" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="R998" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S998" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="T998" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="U998" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="999" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C999" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D999" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="M999" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="O999" s="4" t="s">
+        <v>1555</v>
+      </c>
+      <c r="P999" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q999" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="R999" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S999" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="T999" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="U999" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1000" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C1000" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="D1000" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="M1000" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="O1000" t="s">
+        <v>1556</v>
+      </c>
+      <c r="P1000" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q1000" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="R1000" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="S1000" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="T1000" s="1" t="s">
+        <v>1503</v>
+      </c>
+      <c r="U1000" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="1001" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C1001" s="1" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D1001" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="M1001" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="O1001" t="s">
+        <v>1558</v>
+      </c>
+      <c r="P1001" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q1001" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="R1001" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="S1001" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="T1001" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="U1001" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1002" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C1002" s="1" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D1002" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="M1002" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="O1002" t="s">
+        <v>1559</v>
+      </c>
+      <c r="P1002" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q1002" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="R1002" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="S1002" s="1" t="s">
+        <v>1506</v>
+      </c>
+      <c r="T1002" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="U1002" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1003" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C1003" s="1" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D1003" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="M1003" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="O1003" t="s">
+        <v>1560</v>
+      </c>
+      <c r="P1003" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q1003" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="R1003" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="S1003" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="T1003" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="U1003" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="1004" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C1004" s="1" t="s">
+        <v>1563</v>
+      </c>
+      <c r="D1004" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="M1004" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="O1004" t="s">
+        <v>1562</v>
+      </c>
+      <c r="P1004" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q1004" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="R1004" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1004" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="T1004" s="1" t="s">
+        <v>1507</v>
+      </c>
+      <c r="U1004" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="1005" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C1005" s="1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="D1005" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="M1005" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="O1005" t="s">
+        <v>1564</v>
+      </c>
+      <c r="P1005" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q1005" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="R1005" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="S1005" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="T1005" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="U1005" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="1006" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C1006" s="1" t="s">
+        <v>1567</v>
+      </c>
+      <c r="D1006" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="O1006" t="s">
+        <v>1566</v>
+      </c>
+      <c r="P1006" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q1006" s="1" t="s">
+        <v>1507</v>
+      </c>
+      <c r="R1006" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="S1006" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="T1006" s="1" t="s">
+        <v>1506</v>
+      </c>
+      <c r="U1006" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1007" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="M1007" s="1" t="s">
+        <v>1569</v>
+      </c>
+      <c r="O1007" t="s">
+        <v>1568</v>
+      </c>
+      <c r="P1007" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q1007" s="1" t="s">
+        <v>1505</v>
+      </c>
+      <c r="R1007" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1007" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="T1007" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="U1007" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1008" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="O1008" t="s">
+        <v>1570</v>
+      </c>
+      <c r="P1008" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q1008" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="R1008" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1008" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="T1008" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="U1008" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="1009" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="O1009" t="s">
+        <v>1571</v>
+      </c>
+      <c r="P1009" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q1009" s="1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="R1009" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="S1009" s="1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="T1009" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="U1009" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1010" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C1010" s="1" t="s">
+        <v>1577</v>
+      </c>
+      <c r="D1010" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="M1010" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="O1010" t="s">
+        <v>1573</v>
+      </c>
+      <c r="P1010" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q1010" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="R1010" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="S1010" s="1" t="s">
+        <v>1576</v>
+      </c>
+      <c r="T1010" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="U1010" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="1011" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C1011" s="1" t="s">
+        <v>1577</v>
+      </c>
+      <c r="D1011" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="O1011" t="s">
+        <v>1574</v>
+      </c>
+      <c r="P1011" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="1012" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C1012" s="1" t="s">
+        <v>1577</v>
+      </c>
+      <c r="D1012" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="O1012" t="s">
+        <v>1575</v>
+      </c>
+      <c r="P1012" s="1" t="s">
+        <v>534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>